<commit_message>
new after bucketing and partitioning
</commit_message>
<xml_diff>
--- a/Linux commands.xlsx
+++ b/Linux commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shashankjain/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shashankjain/Desktop/Imp_notes/Summary_notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25B6746-541F-B14E-B3B2-0C2301663ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B76C37-BD27-8E4F-B766-65C20E5BF17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{3284BE38-9AAF-AA4C-96DF-D9DDDFFD684D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{3284BE38-9AAF-AA4C-96DF-D9DDDFFD684D}"/>
   </bookViews>
   <sheets>
     <sheet name="Linux Comands" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="278">
   <si>
     <t>Command</t>
   </si>
@@ -565,9 +565,6 @@
     <t>ctrl u</t>
   </si>
   <si>
-    <t>To delete the line where cursor is</t>
-  </si>
-  <si>
     <t>cmd d</t>
   </si>
   <si>
@@ -851,6 +848,30 @@
   </si>
   <si>
     <t xml:space="preserve">will be log in and in a home directroy. </t>
+  </si>
+  <si>
+    <t>ctrl + k</t>
+  </si>
+  <si>
+    <t>To delete further in the line. Whereever is your cursor is.</t>
+  </si>
+  <si>
+    <t>ctrl k</t>
+  </si>
+  <si>
+    <t>To delete the line before  where cursor is (opposite of ctrl + k)</t>
+  </si>
+  <si>
+    <t>count the number of lines in a file</t>
+  </si>
+  <si>
+    <t>wc -l &lt;name of file&gt;</t>
+  </si>
+  <si>
+    <t>wc &lt;name of file&gt;</t>
+  </si>
+  <si>
+    <t>will give 3 values 1) no. of lines 2)no. words 3) bytes in file</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1299,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B149"/>
+  <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,10 +1361,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1420,18 +1441,18 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1492,18 +1513,18 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1811,7 +1832,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>112</v>
@@ -1952,18 +1973,18 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="96" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B96" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -2013,10 +2034,10 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -2066,50 +2087,50 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
@@ -2118,56 +2139,56 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B126"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B133" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2175,39 +2196,39 @@
         <v>10</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -2217,39 +2238,55 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>266</v>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -2262,57 +2299,63 @@
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" t="s">
         <v>183</v>
-      </c>
-      <c r="B4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
         <v>185</v>
-      </c>
-      <c r="B5" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" t="s">
         <v>187</v>
-      </c>
-      <c r="B6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" t="s">
         <v>189</v>
       </c>
-      <c r="B7" t="s">
-        <v>190</v>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2325,60 +2368,68 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="B1" t="s">
-        <v>175</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" t="s">
         <v>243</v>
-      </c>
-      <c r="B6" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2405,74 +2456,74 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
         <v>223</v>
-      </c>
-      <c r="B2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" t="s">
         <v>226</v>
-      </c>
-      <c r="B5" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" t="s">
         <v>231</v>
-      </c>
-      <c r="B10" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" t="s">
         <v>233</v>
-      </c>
-      <c r="B13" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" t="s">
         <v>235</v>
-      </c>
-      <c r="B14" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" t="s">
         <v>237</v>
-      </c>
-      <c r="B15" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>